<commit_message>
added IRP 2019 costs (error infeasible/unbounded model)
</commit_message>
<xml_diff>
--- a/model_file.xlsx
+++ b/model_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="model_setup" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,6 +44,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Peter Klein
 </t>
@@ -54,6 +55,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Excludes pumping
 Demand increased 1/0.98 for Sasol generation which is not accounted for by Eskom</t>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4634" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4628" uniqueCount="326">
   <si>
     <t xml:space="preserve">wildcard</t>
   </si>
@@ -1067,6 +1069,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1088,6 +1091,7 @@
       <color rgb="FF236194"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1095,12 +1099,14 @@
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1108,6 +1114,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1115,6 +1122,7 @@
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1122,24 +1130,28 @@
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="15">
@@ -2366,6 +2378,7 @@
     <dxf>
       <font>
         <name val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF006100"/>
         <sz val="11"/>
@@ -2379,6 +2392,7 @@
     <dxf>
       <font>
         <name val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF9C5700"/>
         <sz val="11"/>
@@ -2392,6 +2406,7 @@
     <dxf>
       <font>
         <name val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF006100"/>
         <sz val="11"/>
@@ -2405,6 +2420,7 @@
     <dxf>
       <font>
         <name val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF9C5700"/>
         <sz val="11"/>
@@ -2418,6 +2434,7 @@
     <dxf>
       <font>
         <name val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF006100"/>
         <sz val="11"/>
@@ -2431,6 +2448,7 @@
     <dxf>
       <font>
         <name val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF9C5700"/>
         <sz val="11"/>
@@ -2538,8 +2556,8 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2837,7 +2855,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>10</v>
@@ -27872,12 +27890,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI80"/>
+  <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E72" activeCellId="0" sqref="E72"/>
+      <selection pane="bottomLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33859,60 +33877,138 @@
       <c r="A66" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="B66" s="105" t="s">
+      <c r="B66" s="111" t="s">
         <v>256</v>
       </c>
-      <c r="C66" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="D66" s="106" t="n">
-        <v>0</v>
-      </c>
-      <c r="E66" s="106" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" s="106" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" s="106" t="n">
-        <v>0</v>
-      </c>
-      <c r="H66" s="106" t="n">
-        <v>0</v>
-      </c>
-      <c r="I66" s="106" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" s="106" t="n">
-        <v>0</v>
-      </c>
-      <c r="K66" s="106" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" s="106"/>
-      <c r="M66" s="106"/>
-      <c r="N66" s="106"/>
-      <c r="O66" s="106"/>
-      <c r="P66" s="108"/>
-      <c r="Q66" s="108"/>
-      <c r="R66" s="108"/>
-      <c r="S66" s="108"/>
-      <c r="T66" s="108"/>
-      <c r="U66" s="108"/>
-      <c r="V66" s="108"/>
-      <c r="W66" s="108"/>
-      <c r="X66" s="108"/>
-      <c r="Y66" s="108"/>
-      <c r="Z66" s="108"/>
-      <c r="AA66" s="108"/>
-      <c r="AB66" s="108"/>
-      <c r="AC66" s="108"/>
-      <c r="AD66" s="108"/>
-      <c r="AE66" s="108"/>
-      <c r="AF66" s="108"/>
-      <c r="AG66" s="108"/>
-      <c r="AH66" s="108"/>
-      <c r="AI66" s="109"/>
+      <c r="C66" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="D66" s="108" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="108" t="n">
+        <f aca="false">D66</f>
+        <v>0</v>
+      </c>
+      <c r="F66" s="108" t="n">
+        <f aca="false">E66</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="108" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="108" t="n">
+        <f aca="false">G66</f>
+        <v>0</v>
+      </c>
+      <c r="I66" s="108" t="n">
+        <f aca="false">H66</f>
+        <v>0</v>
+      </c>
+      <c r="J66" s="108" t="n">
+        <f aca="false">I66</f>
+        <v>0</v>
+      </c>
+      <c r="K66" s="108" t="n">
+        <f aca="false">J66</f>
+        <v>0</v>
+      </c>
+      <c r="L66" s="108" t="n">
+        <f aca="false">K66</f>
+        <v>0</v>
+      </c>
+      <c r="M66" s="108" t="n">
+        <f aca="false">L66</f>
+        <v>0</v>
+      </c>
+      <c r="N66" s="108" t="n">
+        <f aca="false">M66</f>
+        <v>0</v>
+      </c>
+      <c r="O66" s="108" t="n">
+        <f aca="false">N66</f>
+        <v>0</v>
+      </c>
+      <c r="P66" s="108" t="n">
+        <f aca="false">O66</f>
+        <v>0</v>
+      </c>
+      <c r="Q66" s="108" t="n">
+        <f aca="false">P66</f>
+        <v>0</v>
+      </c>
+      <c r="R66" s="108" t="n">
+        <f aca="false">Q66</f>
+        <v>0</v>
+      </c>
+      <c r="S66" s="108" t="n">
+        <f aca="false">R66</f>
+        <v>0</v>
+      </c>
+      <c r="T66" s="108" t="n">
+        <f aca="false">S66</f>
+        <v>0</v>
+      </c>
+      <c r="U66" s="108" t="n">
+        <f aca="false">T66</f>
+        <v>0</v>
+      </c>
+      <c r="V66" s="108" t="n">
+        <f aca="false">U66</f>
+        <v>0</v>
+      </c>
+      <c r="W66" s="108" t="n">
+        <f aca="false">V66</f>
+        <v>0</v>
+      </c>
+      <c r="X66" s="108" t="n">
+        <f aca="false">W66</f>
+        <v>0</v>
+      </c>
+      <c r="Y66" s="108" t="n">
+        <f aca="false">X66</f>
+        <v>0</v>
+      </c>
+      <c r="Z66" s="108" t="n">
+        <f aca="false">Y66</f>
+        <v>0</v>
+      </c>
+      <c r="AA66" s="108" t="n">
+        <f aca="false">Z66</f>
+        <v>0</v>
+      </c>
+      <c r="AB66" s="108" t="n">
+        <f aca="false">AA66</f>
+        <v>0</v>
+      </c>
+      <c r="AC66" s="108" t="n">
+        <f aca="false">AB66</f>
+        <v>0</v>
+      </c>
+      <c r="AD66" s="108" t="n">
+        <f aca="false">AC66</f>
+        <v>0</v>
+      </c>
+      <c r="AE66" s="108" t="n">
+        <f aca="false">AD66</f>
+        <v>0</v>
+      </c>
+      <c r="AF66" s="108" t="n">
+        <f aca="false">AE66</f>
+        <v>0</v>
+      </c>
+      <c r="AG66" s="108" t="n">
+        <f aca="false">AF66</f>
+        <v>0</v>
+      </c>
+      <c r="AH66" s="108" t="n">
+        <f aca="false">AG66</f>
+        <v>0</v>
+      </c>
+      <c r="AI66" s="110" t="n">
+        <f aca="false">AH66</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="131" t="s">
@@ -33922,133 +34018,103 @@
         <v>256</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>222</v>
+        <v>99</v>
       </c>
       <c r="D67" s="108" t="n">
         <v>0</v>
       </c>
       <c r="E67" s="108" t="n">
-        <f aca="false">D67</f>
         <v>0</v>
       </c>
       <c r="F67" s="108" t="n">
-        <f aca="false">E67</f>
         <v>0</v>
       </c>
       <c r="G67" s="108" t="n">
         <v>0</v>
       </c>
       <c r="H67" s="108" t="n">
-        <f aca="false">G67</f>
         <v>0</v>
       </c>
       <c r="I67" s="108" t="n">
-        <f aca="false">H67</f>
         <v>0</v>
       </c>
       <c r="J67" s="108" t="n">
-        <f aca="false">I67</f>
         <v>0</v>
       </c>
       <c r="K67" s="108" t="n">
-        <f aca="false">J67</f>
         <v>0</v>
       </c>
       <c r="L67" s="108" t="n">
-        <f aca="false">K67</f>
         <v>0</v>
       </c>
       <c r="M67" s="108" t="n">
-        <f aca="false">L67</f>
         <v>0</v>
       </c>
       <c r="N67" s="108" t="n">
-        <f aca="false">M67</f>
         <v>0</v>
       </c>
       <c r="O67" s="108" t="n">
-        <f aca="false">N67</f>
         <v>0</v>
       </c>
       <c r="P67" s="108" t="n">
-        <f aca="false">O67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="Q67" s="108" t="n">
-        <f aca="false">P67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="R67" s="108" t="n">
-        <f aca="false">Q67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="S67" s="108" t="n">
-        <f aca="false">R67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="T67" s="108" t="n">
-        <f aca="false">S67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="U67" s="108" t="n">
-        <f aca="false">T67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="V67" s="108" t="n">
-        <f aca="false">U67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="W67" s="108" t="n">
-        <f aca="false">V67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="X67" s="108" t="n">
-        <f aca="false">W67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="Y67" s="108" t="n">
-        <f aca="false">X67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="Z67" s="108" t="n">
-        <f aca="false">Y67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AA67" s="108" t="n">
-        <f aca="false">Z67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AB67" s="108" t="n">
-        <f aca="false">AA67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AC67" s="108" t="n">
-        <f aca="false">AB67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AD67" s="108" t="n">
-        <f aca="false">AC67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AE67" s="108" t="n">
-        <f aca="false">AD67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AF67" s="108" t="n">
-        <f aca="false">AE67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AG67" s="108" t="n">
-        <f aca="false">AF67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AH67" s="108" t="n">
-        <f aca="false">AG67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AI67" s="110" t="n">
-        <f aca="false">AH67</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34058,260 +34124,260 @@
       <c r="B68" s="111" t="s">
         <v>256</v>
       </c>
-      <c r="C68" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="E68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="F68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="G68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="H68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="I68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="J68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="K68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="L68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="M68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="N68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="O68" s="108" t="n">
-        <v>0</v>
-      </c>
-      <c r="P68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="Q68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="R68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="S68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="T68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="U68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="V68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="W68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="X68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="Y68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="Z68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AA68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AB68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AC68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AD68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AE68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AF68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AG68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AH68" s="108" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AI68" s="110" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="51" t="s">
+        <v>259</v>
+      </c>
+      <c r="D68" s="112" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" s="112" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" s="112" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" s="112"/>
+      <c r="H68" s="112"/>
+      <c r="I68" s="112"/>
+      <c r="J68" s="112"/>
+      <c r="K68" s="112"/>
+      <c r="L68" s="112"/>
+      <c r="M68" s="112"/>
+      <c r="N68" s="112"/>
+      <c r="O68" s="112"/>
+      <c r="P68" s="112"/>
+      <c r="Q68" s="112"/>
+      <c r="R68" s="112"/>
+      <c r="S68" s="112"/>
+      <c r="T68" s="112"/>
+      <c r="U68" s="112"/>
+      <c r="V68" s="112"/>
+      <c r="W68" s="112"/>
+      <c r="X68" s="112"/>
+      <c r="Y68" s="112"/>
+      <c r="Z68" s="112"/>
+      <c r="AA68" s="112"/>
+      <c r="AB68" s="112"/>
+      <c r="AC68" s="112"/>
+      <c r="AD68" s="112"/>
+      <c r="AE68" s="112"/>
+      <c r="AF68" s="112"/>
+      <c r="AG68" s="112"/>
+      <c r="AH68" s="112"/>
+      <c r="AI68" s="113"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="111" t="s">
-        <v>256</v>
-      </c>
-      <c r="C69" s="51" t="s">
-        <v>259</v>
-      </c>
-      <c r="D69" s="112" t="n">
-        <v>0</v>
-      </c>
-      <c r="E69" s="112" t="n">
-        <v>0</v>
-      </c>
-      <c r="F69" s="112" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" s="112"/>
-      <c r="H69" s="112"/>
-      <c r="I69" s="112"/>
-      <c r="J69" s="112"/>
-      <c r="K69" s="112"/>
-      <c r="L69" s="112"/>
-      <c r="M69" s="112"/>
-      <c r="N69" s="112"/>
-      <c r="O69" s="112"/>
-      <c r="P69" s="112"/>
-      <c r="Q69" s="112"/>
-      <c r="R69" s="112"/>
-      <c r="S69" s="112"/>
-      <c r="T69" s="112"/>
-      <c r="U69" s="112"/>
-      <c r="V69" s="112"/>
-      <c r="W69" s="112"/>
-      <c r="X69" s="112"/>
-      <c r="Y69" s="112"/>
-      <c r="Z69" s="112"/>
-      <c r="AA69" s="112"/>
-      <c r="AB69" s="112"/>
-      <c r="AC69" s="112"/>
-      <c r="AD69" s="112"/>
-      <c r="AE69" s="112"/>
-      <c r="AF69" s="112"/>
-      <c r="AG69" s="112"/>
-      <c r="AH69" s="112"/>
-      <c r="AI69" s="113"/>
+      <c r="B69" s="114" t="s">
+        <v>260</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D69" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" s="123" t="n">
+        <v>670</v>
+      </c>
+      <c r="K69" s="123" t="n">
+        <v>1670</v>
+      </c>
+      <c r="L69" s="123" t="n">
+        <v>2670</v>
+      </c>
+      <c r="M69" s="123" t="n">
+        <v>3670</v>
+      </c>
+      <c r="N69" s="123" t="n">
+        <v>4670</v>
+      </c>
+      <c r="O69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="P69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="Q69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="R69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="S69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="T69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="U69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="V69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="W69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="X69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="Y69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="Z69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="AA69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="AB69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="AC69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="AD69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="AE69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="AF69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="AG69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="AH69" s="124" t="n">
+        <v>5670</v>
+      </c>
+      <c r="AI69" s="124" t="n">
+        <v>5670</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="B70" s="114" t="s">
+      <c r="B70" s="115" t="s">
         <v>260</v>
       </c>
-      <c r="C70" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D70" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="E70" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="F70" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="G70" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="H70" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="I70" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="J70" s="123" t="n">
-        <v>670</v>
-      </c>
-      <c r="K70" s="123" t="n">
-        <v>1670</v>
-      </c>
-      <c r="L70" s="123" t="n">
-        <v>2670</v>
-      </c>
-      <c r="M70" s="123" t="n">
-        <v>3670</v>
-      </c>
-      <c r="N70" s="123" t="n">
-        <v>4670</v>
-      </c>
-      <c r="O70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="P70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="Q70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="R70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="S70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="T70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="U70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="V70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="W70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="X70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="Y70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="Z70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="AA70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="AB70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="AC70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="AD70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="AE70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="AF70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="AG70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="AH70" s="124" t="n">
-        <v>5670</v>
-      </c>
-      <c r="AI70" s="124" t="n">
-        <v>5670</v>
+      <c r="C70" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="K70" s="0" t="n">
+        <v>1700</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <v>3300</v>
+      </c>
+      <c r="M70" s="0" t="n">
+        <v>4900</v>
+      </c>
+      <c r="N70" s="0" t="n">
+        <v>6500</v>
+      </c>
+      <c r="O70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="P70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="Q70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="R70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="S70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="T70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="U70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="V70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="W70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="X70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="Y70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="Z70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="AA70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="AB70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="AC70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="AD70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="AE70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="AF70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="AG70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="AH70" s="132" t="n">
+        <v>8100</v>
+      </c>
+      <c r="AI70" s="132" t="n">
+        <v>8100</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34322,7 +34388,7 @@
         <v>260</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>95</v>
+        <v>257</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>0</v>
@@ -34342,82 +34408,82 @@
       <c r="I71" s="132" t="n">
         <v>0</v>
       </c>
-      <c r="J71" s="0" t="n">
-        <v>200</v>
+      <c r="J71" s="132" t="n">
+        <v>0</v>
       </c>
       <c r="K71" s="0" t="n">
-        <v>1700</v>
+        <v>2250</v>
       </c>
       <c r="L71" s="0" t="n">
-        <v>3300</v>
+        <v>3450</v>
       </c>
       <c r="M71" s="0" t="n">
-        <v>4900</v>
+        <v>5250</v>
       </c>
       <c r="N71" s="0" t="n">
-        <v>6500</v>
-      </c>
-      <c r="O71" s="132" t="n">
         <v>8100</v>
       </c>
-      <c r="P71" s="132" t="n">
+      <c r="O71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="Q71" s="132" t="n">
+      <c r="P71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="R71" s="132" t="n">
+      <c r="Q71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="S71" s="132" t="n">
+      <c r="R71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="T71" s="132" t="n">
+      <c r="S71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="U71" s="132" t="n">
+      <c r="T71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="V71" s="132" t="n">
+      <c r="U71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="W71" s="132" t="n">
+      <c r="V71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="X71" s="132" t="n">
+      <c r="W71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="Y71" s="132" t="n">
+      <c r="X71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="Z71" s="132" t="n">
+      <c r="Y71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="AA71" s="132" t="n">
+      <c r="Z71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="AB71" s="132" t="n">
+      <c r="AA71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="AC71" s="132" t="n">
+      <c r="AB71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="AD71" s="132" t="n">
+      <c r="AC71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="AE71" s="132" t="n">
+      <c r="AD71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="AF71" s="132" t="n">
+      <c r="AE71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="AG71" s="132" t="n">
+      <c r="AF71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="AH71" s="132" t="n">
+      <c r="AG71" s="0" t="n">
         <v>8100</v>
       </c>
-      <c r="AI71" s="132" t="n">
+      <c r="AH71" s="0" t="n">
+        <v>8100</v>
+      </c>
+      <c r="AI71" s="0" t="n">
         <v>8100</v>
       </c>
     </row>
@@ -34429,7 +34495,7 @@
         <v>260</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>0</v>
@@ -34452,80 +34518,80 @@
       <c r="J72" s="132" t="n">
         <v>0</v>
       </c>
-      <c r="K72" s="0" t="n">
-        <v>2250</v>
-      </c>
-      <c r="L72" s="0" t="n">
-        <v>3450</v>
-      </c>
-      <c r="M72" s="0" t="n">
-        <v>5250</v>
-      </c>
-      <c r="N72" s="0" t="n">
-        <v>8100</v>
-      </c>
-      <c r="O72" s="0" t="n">
-        <v>8100</v>
+      <c r="K72" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="L72" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="N72" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="O72" s="132" t="n">
+        <v>0</v>
       </c>
       <c r="P72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="Q72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="R72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="S72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="T72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="U72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="V72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="W72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="X72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="Y72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="Z72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="AA72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="AB72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="AC72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="AD72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="AE72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="AF72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="AG72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="AH72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
       <c r="AI72" s="0" t="n">
-        <v>8100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34536,7 +34602,7 @@
         <v>260</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>258</v>
+        <v>167</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>0</v>
@@ -34643,7 +34709,7 @@
         <v>260</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>167</v>
+        <v>60</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>0</v>
@@ -34657,89 +34723,89 @@
       <c r="G74" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H74" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="I74" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="J74" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="K74" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="L74" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="M74" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="N74" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="O74" s="132" t="n">
-        <v>0</v>
+      <c r="H74" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J74" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K74" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L74" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M74" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N74" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O74" s="0" t="n">
+        <v>1000</v>
       </c>
       <c r="P74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="Q74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="R74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="S74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="T74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="U74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="V74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="W74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="X74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="Y74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="Z74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AA74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AB74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AC74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AD74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AE74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AF74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AG74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AH74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AI74" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34750,7 +34816,7 @@
         <v>260</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>0</v>
@@ -34764,89 +34830,89 @@
       <c r="G75" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H75" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="I75" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J75" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="K75" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L75" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M75" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="N75" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O75" s="0" t="n">
-        <v>1000</v>
+      <c r="H75" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="L75" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="M75" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="N75" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="O75" s="132" t="n">
+        <v>0</v>
       </c>
       <c r="P75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI75" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34857,7 +34923,7 @@
         <v>260</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>97</v>
+        <v>222</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -34960,11 +35026,11 @@
       <c r="A77" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="B77" s="115" t="s">
+      <c r="B77" s="133" t="s">
         <v>260</v>
       </c>
-      <c r="C77" s="0" t="s">
-        <v>104</v>
+      <c r="C77" s="24" t="s">
+        <v>99</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>0</v>
@@ -34978,414 +35044,202 @@
       <c r="G77" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H77" s="0" t="n">
+      <c r="H77" s="132" t="n">
         <v>0</v>
       </c>
       <c r="I77" s="132" t="n">
         <v>0</v>
       </c>
-      <c r="J77" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K77" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L77" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M77" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N77" s="0" t="n">
+      <c r="J77" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="L77" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" s="132" t="n">
+        <v>0</v>
+      </c>
+      <c r="N77" s="132" t="n">
         <v>0</v>
       </c>
       <c r="O77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="P77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="Q77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="R77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="S77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="T77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="U77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="V77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="W77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="X77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="Y77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="Z77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="AA77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="AB77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="AC77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="AD77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="AE77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="AF77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="AG77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="AH77" s="132" t="n">
-        <v>2500</v>
-      </c>
-      <c r="AI77" s="132" t="n">
-        <v>2500</v>
+        <v>0</v>
+      </c>
+      <c r="P77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI77" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="B78" s="115" t="s">
+      <c r="B78" s="118" t="s">
         <v>260</v>
       </c>
-      <c r="C78" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="D78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H78" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="I78" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="J78" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="K78" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="L78" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="M78" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="N78" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="O78" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="P78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI78" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="131" t="s">
-        <v>30</v>
-      </c>
-      <c r="B79" s="133" t="s">
-        <v>260</v>
-      </c>
-      <c r="C79" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H79" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="I79" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="K79" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="L79" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="M79" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="N79" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="O79" s="132" t="n">
-        <v>0</v>
-      </c>
-      <c r="P79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI79" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="131" t="s">
-        <v>30</v>
-      </c>
-      <c r="B80" s="118" t="s">
-        <v>260</v>
-      </c>
-      <c r="C80" s="51" t="s">
+      <c r="C78" s="51" t="s">
         <v>259</v>
       </c>
-      <c r="D80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="E80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="F80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="G80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="H80" s="135" t="n">
-        <v>0</v>
-      </c>
-      <c r="I80" s="135" t="n">
-        <v>0</v>
-      </c>
-      <c r="J80" s="135" t="n">
-        <v>0</v>
-      </c>
-      <c r="K80" s="135" t="n">
-        <v>0</v>
-      </c>
-      <c r="L80" s="135" t="n">
-        <v>0</v>
-      </c>
-      <c r="M80" s="135" t="n">
-        <v>0</v>
-      </c>
-      <c r="N80" s="135" t="n">
-        <v>0</v>
-      </c>
-      <c r="O80" s="135" t="n">
-        <v>0</v>
-      </c>
-      <c r="P80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="R80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="S80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="T80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="U80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="V80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="W80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="X80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH80" s="134" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI80" s="134" t="n">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="D78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="135" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" s="135" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="135" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" s="135" t="n">
+        <v>0</v>
+      </c>
+      <c r="L78" s="135" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" s="135" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" s="135" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" s="135" t="n">
+        <v>0</v>
+      </c>
+      <c r="P78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="R78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="S78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="T78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="U78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="V78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="W78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="X78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH78" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI78" s="134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="D31:F36 D9:AI10 D50:F55 D12:AI20 G52:AI55 D56:AI58 D47:AI47 G33:AI36 D37:AI39 D67:AI68">
+  <conditionalFormatting sqref="D31:F36 D9:AI10 D50:F55 D12:AI20 G52:AI55 D56:AI58 D47:AI47 G33:AI36 D37:AI39 D66:AI67">
     <cfRule type="cellIs" priority="2" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>0</formula>
     </cfRule>
@@ -35401,7 +35255,7 @@
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:AI11 D26:AI30 D7:AI8 D48:AI49 D45:AI46 D69:AI69 D65:AI66">
+  <conditionalFormatting sqref="D11:AI11 D26:AI30 D7:AI8 D48:AI49 D45:AI46 D68:AI68 D65:AI65">
     <cfRule type="cellIs" priority="6" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>0</formula>
     </cfRule>

</xml_diff>